<commit_message>
Add Error to review template
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation_process/input/annotation_full_review_template.xlsx
+++ b/brise_plandok/annotation_process/input/annotation_full_review_template.xlsx
@@ -22,6 +22,7 @@
     <definedName function="false" hidden="false" name="Hoehe" vbProcedure="false">Label!$H$4:$H$12</definedName>
     <definedName function="false" hidden="false" name="Lage_Gelaende_Planzeichen" vbProcedure="false">Label!$S$4:$S$11</definedName>
     <definedName function="false" hidden="false" name="Laubengaenge_Durchfahrten_Arkaden" vbProcedure="false">Label!$O$4:$O$11</definedName>
+    <definedName function="false" hidden="false" name="Meta" vbProcedure="false">Label!$T$4</definedName>
     <definedName function="false" hidden="false" name="Modality" vbProcedure="false">Label!$X$4:$X$6</definedName>
     <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$M$4:$M$10</definedName>
     <definedName function="false" hidden="false" name="Sentence_Review" vbProcedure="false">Label!$Z$4:$Z$5</definedName>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -117,6 +118,9 @@
     <t xml:space="preserve">Lage_Gelaende_Planzeichen</t>
   </si>
   <si>
+    <t xml:space="preserve">Meta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sentence Review</t>
   </si>
   <si>
@@ -162,6 +166,9 @@
     <t xml:space="preserve">AnFluchtlinie</t>
   </si>
   <si>
+    <t xml:space="preserve">Error</t>
+  </si>
+  <si>
     <t xml:space="preserve">content</t>
   </si>
   <si>
@@ -406,9 +413,6 @@
   </si>
   <si>
     <t xml:space="preserve">ErrichtungGebaeude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meta</t>
   </si>
   <si>
     <t xml:space="preserve">VerbotStellplaetzeUndParkgebaeude</t>
@@ -448,9 +452,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -594,43 +599,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -642,7 +647,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1278,10 +1283,10 @@
   <dimension ref="B1:Z24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA9" activeCellId="0" sqref="AA9"/>
+      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1362,7 +1367,9 @@
       <c r="S3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="11"/>
+      <c r="T3" s="11" t="s">
+        <v>24</v>
+      </c>
       <c r="U3" s="11" t="s">
         <v>8</v>
       </c>
@@ -1370,7 +1377,7 @@
         <v>3</v>
       </c>
       <c r="Z3" s="12" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1378,55 +1385,58 @@
         <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
+      </c>
+      <c r="T4" s="0" t="s">
+        <v>40</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1434,49 +1444,49 @@
         <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="X5" s="13" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1484,46 +1494,46 @@
         <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1531,37 +1541,37 @@
         <v>15</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1569,34 +1579,34 @@
         <v>23</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1604,28 +1614,28 @@
         <v>21</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1633,25 +1643,25 @@
         <v>19</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,22 +1669,22 @@
         <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1682,13 +1692,13 @@
         <v>22</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1696,13 +1706,13 @@
         <v>13</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1710,67 +1720,67 @@
         <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="11" t="s">
-        <v>121</v>
+        <v>24</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11"/>
       <c r="P16" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split Flaechen to 4 subcategories
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation_process/input/annotation_full_review_template.xlsx
+++ b/brise_plandok/annotation_process/input/annotation_full_review_template.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$15</definedName>
     <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$24</definedName>
-    <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$12</definedName>
+    <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$11</definedName>
     <definedName function="false" hidden="false" name="Einfriedungen" vbProcedure="false">Label!$L$4:$L$8</definedName>
-    <definedName function="false" hidden="false" name="Flaeche" vbProcedure="false">Label!$G$4:$G$4</definedName>
+    <definedName function="false" hidden="false" name="Flaeche" vbProcedure="false">Label!$G$4:$G$8</definedName>
     <definedName function="false" hidden="false" name="Geschosse" vbProcedure="false">Label!$J$4:$J$9</definedName>
     <definedName function="false" hidden="false" name="Grossbauvorhaben_Hochhaeuser_Einkaufszentren_Geschaeftsgebaeude" vbProcedure="false">Label!$N$4:$N$6</definedName>
-    <definedName function="false" hidden="false" name="Hoehe" vbProcedure="false">Label!$H$4:$H$12</definedName>
+    <definedName function="false" hidden="false" name="Hoehe" vbProcedure="false">Label!$H$4:$H$13</definedName>
     <definedName function="false" hidden="false" name="Lage_Gelaende_Planzeichen" vbProcedure="false">Label!$S$4:$S$11</definedName>
     <definedName function="false" hidden="false" name="Laubengaenge_Durchfahrten_Arkaden" vbProcedure="false">Label!$O$4:$O$11</definedName>
     <definedName function="false" hidden="false" name="Meta" vbProcedure="false">Label!$T$4</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="138">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -178,6 +178,9 @@
     <t xml:space="preserve">Done</t>
   </si>
   <si>
+    <t xml:space="preserve">BebauteFlaecheMax</t>
+  </si>
+  <si>
     <t xml:space="preserve">BauklasseVIHoeheMax</t>
   </si>
   <si>
@@ -223,6 +226,9 @@
     <t xml:space="preserve">Question</t>
   </si>
   <si>
+    <t xml:space="preserve">BebauteFlaecheMaxProzentual</t>
+  </si>
+  <si>
     <t xml:space="preserve">BauklasseVIHoeheMin</t>
   </si>
   <si>
@@ -265,6 +271,9 @@
     <t xml:space="preserve">prohibition</t>
   </si>
   <si>
+    <t xml:space="preserve">BebauteFlaecheMaxNebengebaeude</t>
+  </si>
+  <si>
     <t xml:space="preserve">FBOKMinimumWohnungen</t>
   </si>
   <si>
@@ -296,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">conditionException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BebauteFlaecheMin</t>
   </si>
   <si>
     <t xml:space="preserve">GebaeudeHoeheArt</t>
@@ -594,7 +606,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -645,6 +657,10 @@
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -1282,11 +1298,11 @@
   </sheetPr>
   <dimension ref="B1:Z24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="S1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T8" activeCellId="0" sqref="T8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1443,170 +1459,182 @@
       <c r="B5" s="11" t="s">
         <v>17</v>
       </c>
+      <c r="G5" s="13" t="s">
+        <v>44</v>
+      </c>
       <c r="H5" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="X5" s="13" t="s">
         <v>57</v>
       </c>
+      <c r="X5" s="14" t="s">
+        <v>58</v>
+      </c>
       <c r="Z5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="11" t="s">
         <v>20</v>
       </c>
+      <c r="G6" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="H6" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="11" t="s">
         <v>15</v>
       </c>
+      <c r="G7" s="13" t="s">
+        <v>75</v>
+      </c>
       <c r="H7" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
+      <c r="G8" s="13" t="s">
+        <v>87</v>
+      </c>
       <c r="H8" s="0" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1614,28 +1642,28 @@
         <v>21</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1643,25 +1671,25 @@
         <v>19</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1669,22 +1697,22 @@
         <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1692,13 +1720,13 @@
         <v>22</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,13 +1734,13 @@
         <v>13</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,10 +1748,10 @@
         <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1731,56 +1759,56 @@
         <v>24</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11"/>
       <c r="P16" s="0" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>127</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="0" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add script for renaming attributes
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation_process/input/annotation_full_review_template.xlsx
+++ b/brise_plandok/annotation_process/input/annotation_full_review_template.xlsx
@@ -16,7 +16,7 @@
     <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$24</definedName>
     <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$11</definedName>
     <definedName function="false" hidden="false" name="Einfriedungen" vbProcedure="false">Label!$L$4:$L$8</definedName>
-    <definedName function="false" hidden="false" name="Flaeche" vbProcedure="false">Label!$G$4:$G$8</definedName>
+    <definedName function="false" hidden="false" name="Flaeche" vbProcedure="false">Label!$G$4:$G$7</definedName>
     <definedName function="false" hidden="false" name="Geschosse" vbProcedure="false">Label!$J$4:$J$9</definedName>
     <definedName function="false" hidden="false" name="Grossbauvorhaben_Hochhaeuser_Einkaufszentren_Geschaeftsgebaeude" vbProcedure="false">Label!$N$4:$N$6</definedName>
     <definedName function="false" hidden="false" name="Hoehe" vbProcedure="false">Label!$H$4:$H$13</definedName>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="137">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">VolumenUndUmbaubarerRaum</t>
   </si>
   <si>
-    <t xml:space="preserve">Flaechen</t>
+    <t xml:space="preserve">BebauteFlaecheMax</t>
   </si>
   <si>
     <t xml:space="preserve">Bauklasse</t>
@@ -178,7 +178,7 @@
     <t xml:space="preserve">Done</t>
   </si>
   <si>
-    <t xml:space="preserve">BebauteFlaecheMax</t>
+    <t xml:space="preserve">BebauteFlaecheMaxProzentual</t>
   </si>
   <si>
     <t xml:space="preserve">BauklasseVIHoeheMax</t>
@@ -226,7 +226,7 @@
     <t xml:space="preserve">Question</t>
   </si>
   <si>
-    <t xml:space="preserve">BebauteFlaecheMaxProzentual</t>
+    <t xml:space="preserve">BebauteFlaecheMaxNebengebaeude</t>
   </si>
   <si>
     <t xml:space="preserve">BauklasseVIHoeheMin</t>
@@ -271,7 +271,7 @@
     <t xml:space="preserve">prohibition</t>
   </si>
   <si>
-    <t xml:space="preserve">BebauteFlaecheMaxNebengebaeude</t>
+    <t xml:space="preserve">BebauteFlaecheMin</t>
   </si>
   <si>
     <t xml:space="preserve">FBOKMinimumWohnungen</t>
@@ -301,43 +301,40 @@
     <t xml:space="preserve">StrassenbreiteMin</t>
   </si>
   <si>
+    <t xml:space="preserve">GesamtePlangebiet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">conditionException</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GebaeudeHoeheArt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StellplatzMax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnterirdischeBaulichkeiten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EinfriedungZulaessig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VerbotWohnung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DurchgangBreite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AufbautenZulaessig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dachart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StrassenbreiteVonBis</t>
+  </si>
+  <si>
     <t xml:space="preserve">InSchutzzone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">conditionException</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BebauteFlaecheMin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GebaeudeHoeheArt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StellplatzMax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UnterirdischeBaulichkeiten</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EinfriedungZulaessig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VerbotWohnung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DurchgangBreite</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AufbautenZulaessig</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dachart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">StrassenbreiteVonBis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PlangebietAllgemein</t>
   </si>
   <si>
     <t xml:space="preserve">GebaeudeHoeheMax</t>
@@ -1298,11 +1295,11 @@
   </sheetPr>
   <dimension ref="B1:Z24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="Q1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.95703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1403,7 +1400,7 @@
       <c r="F4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="G4" s="13" t="s">
         <v>27</v>
       </c>
       <c r="H4" s="0" t="s">
@@ -1592,7 +1589,7 @@
       <c r="R7" s="0" t="s">
         <v>84</v>
       </c>
-      <c r="S7" s="0" t="s">
+      <c r="S7" s="13" t="s">
         <v>85</v>
       </c>
       <c r="U7" s="0" t="s">
@@ -1603,38 +1600,35 @@
       <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="0" t="s">
         <v>87</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>88</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="J8" s="0" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="L8" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="M8" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="M8" s="0" t="s">
+      <c r="O8" s="0" t="s">
         <v>92</v>
       </c>
-      <c r="O8" s="0" t="s">
+      <c r="P8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="0" t="s">
+      <c r="Q8" s="0" t="s">
         <v>94</v>
       </c>
-      <c r="Q8" s="0" t="s">
+      <c r="R8" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="R8" s="0" t="s">
+      <c r="S8" s="0" t="s">
         <v>96</v>
-      </c>
-      <c r="S8" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1642,28 +1636,28 @@
         <v>21</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="J9" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="J9" s="0" t="s">
+      <c r="M9" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="M9" s="0" t="s">
+      <c r="O9" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="O9" s="0" t="s">
+      <c r="P9" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="P9" s="0" t="s">
+      <c r="Q9" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="Q9" s="0" t="s">
+      <c r="S9" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="S9" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1671,25 +1665,25 @@
         <v>19</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="M10" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="O10" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="P10" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="Q10" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="S10" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="S10" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1697,22 +1691,22 @@
         <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="O11" s="0" t="s">
         <v>114</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="P11" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="P11" s="0" t="s">
+      <c r="Q11" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="S11" s="0" t="s">
         <v>117</v>
-      </c>
-      <c r="S11" s="0" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1720,13 +1714,13 @@
         <v>22</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="P12" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1734,13 +1728,13 @@
         <v>13</v>
       </c>
       <c r="H13" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="P13" s="0" t="s">
         <v>123</v>
-      </c>
-      <c r="P13" s="0" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1748,10 +1742,10 @@
         <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="P14" s="0" t="s">
         <v>125</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1759,56 +1753,56 @@
         <v>24</v>
       </c>
       <c r="I15" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="P15" s="0" t="s">
         <v>127</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="11"/>
       <c r="P16" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P24" s="0" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>